<commit_message>
Revert "Merge branch 'main' of https://github.com/matzat5/Ro_Tech"
This reverts commit fc7ad9a8d794aed6d19c3a8005166e985b3d0e12, reversing
changes made to d08dad673db846a2403e813694129bb72e6d01f3.
</commit_message>
<xml_diff>
--- a/2. Ссылки на гугл-таблицы, диски и проги/Гугл таблицы для руководителей отделов/1. Результаты отбора/1. Отбор Осень 2024/Лист Microsoft Excel.xlsx
+++ b/2. Ссылки на гугл-таблицы, диски и проги/Гугл таблицы для руководителей отделов/1. Результаты отбора/1. Отбор Осень 2024/Лист Microsoft Excel.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20827"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E5F5F6A7-EA9C-4F43-88A0-B2E54F47FDB3}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6164532A-EACE-43F1-B13E-CB2E3DEC070E}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="29">
   <si>
     <t>Фамилия</t>
   </si>
@@ -107,42 +107,6 @@
   </si>
   <si>
     <t>Вставили ссылки, секс</t>
-  </si>
-  <si>
-    <t>Дьяков</t>
-  </si>
-  <si>
-    <t>Да, исп в электронике</t>
-  </si>
-  <si>
-    <t>Загумённая</t>
-  </si>
-  <si>
-    <t>Юнг</t>
-  </si>
-  <si>
-    <t>Чашин</t>
-  </si>
-  <si>
-    <t>Написал расчётную программу на плюсах</t>
-  </si>
-  <si>
-    <t>Цапкин</t>
-  </si>
-  <si>
-    <t>Струнков</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> </t>
-  </si>
-  <si>
-    <t>Окунь</t>
-  </si>
-  <si>
-    <t>Выполнено совмесно с Зубаревой</t>
-  </si>
-  <si>
-    <t>Разберёт полки</t>
   </si>
 </sst>
 </file>
@@ -210,14 +174,14 @@
   </cellStyleXfs>
   <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Обычный" xfId="0" builtinId="0"/>
@@ -498,366 +462,211 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:N23"/>
+  <dimension ref="A1:M14"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="G25" sqref="G25"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C17" sqref="C17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="11.42578125" customWidth="1"/>
-    <col min="3" max="3" width="17" customWidth="1"/>
-    <col min="4" max="4" width="18.5703125" customWidth="1"/>
-    <col min="5" max="5" width="19.140625" customWidth="1"/>
-    <col min="6" max="6" width="19.28515625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="17.28515625" customWidth="1"/>
-    <col min="8" max="8" width="14.5703125" customWidth="1"/>
-    <col min="9" max="9" width="15" customWidth="1"/>
-    <col min="11" max="11" width="43.7109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="11.42578125" customWidth="1"/>
+    <col min="2" max="2" width="17" customWidth="1"/>
+    <col min="3" max="3" width="18.5703125" customWidth="1"/>
+    <col min="4" max="4" width="19.140625" customWidth="1"/>
+    <col min="5" max="5" width="19.28515625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="17.28515625" customWidth="1"/>
+    <col min="7" max="7" width="14.5703125" customWidth="1"/>
+    <col min="8" max="8" width="15" customWidth="1"/>
+    <col min="10" max="10" width="43.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
       <c r="B1" t="s">
-        <v>0</v>
-      </c>
-      <c r="C1" t="s">
         <v>3</v>
       </c>
-      <c r="D1" s="6" t="s">
+      <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="E1" s="6"/>
-      <c r="F1" s="6"/>
-      <c r="G1" s="6" t="s">
+      <c r="D1" s="1"/>
+      <c r="E1" s="1"/>
+      <c r="F1" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="6"/>
-      <c r="I1" t="s">
+      <c r="G1" s="1"/>
+      <c r="H1" t="s">
         <v>9</v>
       </c>
-      <c r="K1" t="s">
+      <c r="J1" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="C2" t="s">
+        <v>4</v>
+      </c>
       <c r="D2" t="s">
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="E2" t="s">
+        <v>5</v>
+      </c>
+      <c r="F2" t="s">
+        <v>7</v>
+      </c>
+      <c r="G2" t="s">
         <v>8</v>
       </c>
-      <c r="F2" t="s">
-        <v>5</v>
-      </c>
-      <c r="G2" t="s">
-        <v>7</v>
-      </c>
-      <c r="H2" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A3">
+    </row>
+    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
         <v>1</v>
       </c>
-      <c r="B3" t="s">
-        <v>1</v>
-      </c>
-      <c r="C3" s="1"/>
+      <c r="B3" s="2"/>
+      <c r="C3" s="3"/>
       <c r="D3" s="2"/>
-      <c r="E3" s="1"/>
-      <c r="F3" s="3"/>
-      <c r="G3" s="1"/>
-      <c r="H3" s="2"/>
-      <c r="I3" s="4"/>
-      <c r="K3" t="s">
+      <c r="E3" s="4"/>
+      <c r="F3" s="2"/>
+      <c r="G3" s="3"/>
+      <c r="H3" s="5"/>
+      <c r="J3" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="4" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A4">
-        <v>2</v>
-      </c>
-      <c r="B4" t="s">
+    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
         <v>10</v>
       </c>
+      <c r="B4" s="5"/>
       <c r="C4" s="4"/>
-      <c r="D4" s="3"/>
-      <c r="E4" s="3"/>
-      <c r="F4" s="3"/>
-      <c r="G4" s="1"/>
-      <c r="H4" s="3"/>
-      <c r="I4" s="3"/>
-      <c r="K4" t="s">
+      <c r="D4" s="4"/>
+      <c r="E4" s="4"/>
+      <c r="F4" s="2"/>
+      <c r="G4" s="4"/>
+      <c r="H4" s="4"/>
+      <c r="J4" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="5" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A5">
-        <v>3</v>
-      </c>
-      <c r="B5" t="s">
+    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
         <v>14</v>
       </c>
-      <c r="C5" s="1"/>
-      <c r="D5" s="1"/>
-      <c r="E5" s="2"/>
-      <c r="F5" s="2"/>
-      <c r="G5" s="3"/>
+      <c r="B5" s="2"/>
+      <c r="C5" s="2"/>
+      <c r="D5" s="3"/>
+      <c r="E5" s="3"/>
+      <c r="F5" s="4"/>
+      <c r="G5" s="4"/>
       <c r="H5" s="3"/>
-      <c r="I5" s="2"/>
+      <c r="J5" t="s">
+        <v>15</v>
+      </c>
       <c r="K5" t="s">
-        <v>15</v>
-      </c>
-      <c r="L5" t="s">
         <v>16</v>
       </c>
-      <c r="M5" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="6" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A6">
-        <v>4</v>
-      </c>
-      <c r="B6" t="s">
+    </row>
+    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
         <v>17</v>
       </c>
-      <c r="C6" s="5"/>
-      <c r="D6" s="3"/>
-      <c r="E6" s="3"/>
-      <c r="F6" s="3"/>
-      <c r="G6" s="5"/>
-      <c r="H6" s="5"/>
-      <c r="I6" s="3"/>
-      <c r="K6" s="4" t="s">
+      <c r="B6" s="6"/>
+      <c r="C6" s="4"/>
+      <c r="D6" s="4"/>
+      <c r="E6" s="4"/>
+      <c r="F6" s="6"/>
+      <c r="G6" s="6"/>
+      <c r="H6" s="4"/>
+      <c r="J6" s="5" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="7" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A7">
-        <v>5</v>
-      </c>
-      <c r="B7" t="s">
+    <row r="7" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
         <v>19</v>
       </c>
-      <c r="C7" s="4"/>
+      <c r="B7" s="5"/>
+      <c r="C7" s="5"/>
       <c r="D7" s="4"/>
-      <c r="E7" s="3"/>
-      <c r="F7" s="3"/>
-      <c r="G7" s="1"/>
-      <c r="H7" s="3"/>
-      <c r="I7" s="3"/>
-    </row>
-    <row r="8" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A8">
-        <v>6</v>
-      </c>
-      <c r="B8" t="s">
+      <c r="E7" s="4"/>
+      <c r="F7" s="2"/>
+      <c r="G7" s="4"/>
+      <c r="H7" s="4"/>
+    </row>
+    <row r="8" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
         <v>20</v>
       </c>
-      <c r="C8" s="1"/>
-      <c r="D8" s="1"/>
-      <c r="E8" s="2"/>
-      <c r="F8" s="4"/>
-      <c r="G8" s="5"/>
-      <c r="H8" s="1"/>
-      <c r="I8" s="5"/>
-      <c r="K8" s="4" t="s">
+      <c r="B8" s="2"/>
+      <c r="C8" s="2"/>
+      <c r="D8" s="3"/>
+      <c r="E8" s="5"/>
+      <c r="F8" s="6"/>
+      <c r="G8" s="2"/>
+      <c r="H8" s="6"/>
+      <c r="J8" s="5" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="9" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A9">
-        <v>7</v>
-      </c>
-      <c r="B9" t="s">
+    <row r="9" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
         <v>22</v>
       </c>
-      <c r="C9" s="1"/>
-      <c r="D9" s="1"/>
-      <c r="E9" s="2"/>
-      <c r="F9" s="3"/>
-      <c r="G9" s="4"/>
-      <c r="H9" s="1"/>
-      <c r="I9" s="4"/>
-      <c r="K9" t="s">
+      <c r="B9" s="2"/>
+      <c r="C9" s="2"/>
+      <c r="D9" s="3"/>
+      <c r="E9" s="4"/>
+      <c r="F9" s="5"/>
+      <c r="G9" s="2"/>
+      <c r="H9" s="5"/>
+      <c r="J9" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="10" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A10">
-        <v>8</v>
-      </c>
-      <c r="B10" t="s">
+    <row r="10" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
         <v>23</v>
       </c>
-      <c r="C10" s="5"/>
-      <c r="D10" s="5"/>
-      <c r="E10" s="1"/>
-      <c r="F10" s="1"/>
-      <c r="G10" s="4"/>
-      <c r="H10" s="1"/>
-      <c r="I10" s="5"/>
-      <c r="K10" s="4" t="s">
+      <c r="B10" s="6"/>
+      <c r="C10" s="6"/>
+      <c r="D10" s="2"/>
+      <c r="E10" s="2"/>
+      <c r="F10" s="5"/>
+      <c r="G10" s="2"/>
+      <c r="H10" s="6"/>
+      <c r="J10" s="5" t="s">
         <v>27</v>
       </c>
-      <c r="N10" s="5"/>
-    </row>
-    <row r="11" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A11">
-        <v>9</v>
-      </c>
-      <c r="B11" t="s">
+      <c r="M10" s="6"/>
+    </row>
+    <row r="11" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
         <v>25</v>
       </c>
-      <c r="C11" s="5"/>
-      <c r="D11" s="5"/>
-      <c r="E11" s="1"/>
-      <c r="F11" s="1"/>
-      <c r="G11" s="4"/>
-      <c r="H11" s="1"/>
-      <c r="I11" s="5"/>
-      <c r="K11" t="s">
+      <c r="J11" t="s">
         <v>28</v>
       </c>
-      <c r="N11" s="4"/>
-    </row>
-    <row r="12" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A12">
-        <v>10</v>
-      </c>
-      <c r="B12" t="s">
+      <c r="M11" s="5"/>
+    </row>
+    <row r="12" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
         <v>26</v>
       </c>
-      <c r="C12" s="5"/>
-      <c r="D12" s="5"/>
-      <c r="E12" s="1"/>
-      <c r="F12" s="1"/>
-      <c r="G12" s="4"/>
-      <c r="H12" s="1"/>
-      <c r="I12" s="5"/>
-      <c r="N12" s="1"/>
-    </row>
-    <row r="13" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A13">
-        <v>11</v>
-      </c>
-      <c r="B13" t="s">
-        <v>29</v>
-      </c>
-      <c r="C13" s="1"/>
-      <c r="D13" s="1"/>
-      <c r="E13" s="2"/>
-      <c r="F13" s="2"/>
-      <c r="G13" s="3"/>
-      <c r="H13" s="3"/>
-      <c r="I13" s="2"/>
-      <c r="K13" t="s">
-        <v>39</v>
-      </c>
-      <c r="N13" s="2"/>
-    </row>
-    <row r="14" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A14">
-        <v>12</v>
-      </c>
-      <c r="B14" t="s">
-        <v>31</v>
-      </c>
-      <c r="C14" s="1"/>
-      <c r="D14" s="4"/>
-      <c r="E14" s="5"/>
-      <c r="F14" s="5"/>
-      <c r="G14" s="3"/>
-      <c r="H14" s="3"/>
-      <c r="I14" s="4"/>
-      <c r="N14" s="3"/>
-    </row>
-    <row r="15" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A15">
-        <v>13</v>
-      </c>
-      <c r="B15" t="s">
-        <v>32</v>
-      </c>
-      <c r="C15" s="2"/>
-      <c r="D15" s="3"/>
-      <c r="E15" s="3"/>
-      <c r="F15" s="3"/>
-      <c r="G15" s="4"/>
-      <c r="H15" s="3"/>
-      <c r="I15" s="3"/>
-    </row>
-    <row r="16" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A16">
-        <v>14</v>
-      </c>
-      <c r="B16" t="s">
-        <v>35</v>
-      </c>
-      <c r="C16" s="2"/>
-      <c r="D16" s="2"/>
-      <c r="E16" s="2"/>
-      <c r="F16" s="2"/>
-      <c r="G16" s="2"/>
-      <c r="H16" s="2"/>
-      <c r="I16" s="2"/>
-    </row>
-    <row r="17" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A17">
-        <v>15</v>
-      </c>
-      <c r="B17" t="s">
-        <v>33</v>
-      </c>
-      <c r="C17" s="5"/>
-      <c r="D17" s="3"/>
-      <c r="E17" s="3"/>
-      <c r="F17" s="3"/>
-      <c r="G17" s="3"/>
-      <c r="H17" s="3"/>
-      <c r="I17" s="3"/>
-      <c r="K17" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="18" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A18">
-        <v>16</v>
-      </c>
-      <c r="B18" t="s">
-        <v>36</v>
-      </c>
-      <c r="C18" s="5"/>
-      <c r="D18" s="1"/>
-      <c r="E18" s="4"/>
-      <c r="F18" s="5"/>
-      <c r="G18" s="1"/>
-      <c r="H18" s="3"/>
-      <c r="I18" s="1"/>
-    </row>
-    <row r="19" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A19">
-        <v>17</v>
-      </c>
-      <c r="B19" t="s">
-        <v>38</v>
-      </c>
-      <c r="K19" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="23" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="D23" t="s">
-        <v>37</v>
-      </c>
+      <c r="M12" s="2"/>
+    </row>
+    <row r="13" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="M13" s="3"/>
+    </row>
+    <row r="14" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="M14" s="4"/>
     </row>
   </sheetData>
   <mergeCells count="2">
-    <mergeCell ref="G1:H1"/>
-    <mergeCell ref="D1:F1"/>
+    <mergeCell ref="F1:G1"/>
+    <mergeCell ref="C1:E1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>